<commit_message>
edit app and input excel
</commit_message>
<xml_diff>
--- a/soal-kunci-clean.xlsx
+++ b/soal-kunci-clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sistem-penilaian-levenshtein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB76CC4-C6B6-4B51-962F-8C3998ADB513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF672CF-9432-4255-902C-49DDDD9A0410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="297">
   <si>
     <t>Soal</t>
   </si>
@@ -442,6 +442,813 @@
   </si>
   <si>
     <t>Sebutkan 5 contoh kata kerja berawalan "me-"!</t>
+  </si>
+  <si>
+    <t>Melompat, memukul, menyapu, mengejar, menonton.</t>
+  </si>
+  <si>
+    <t>Buat kalimat yang menunjukkan aktivitas dengan awalan "mem-"!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ibu sedang </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>memasak</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sayur di dapur.</t>
+    </r>
+  </si>
+  <si>
+    <t>Apa fungsi awalan "di-" dalam kalimat pasif?</t>
+  </si>
+  <si>
+    <t>Awalan "di-" digunakan untuk menyatakan bahwa suatu tindakan diterima atau dilakukan terhadap subjek (kalimat pasif).</t>
+  </si>
+  <si>
+    <t>Tuliskan perbedaan kalimat aktif dan pasif dengan awalan "me-" dan "di-"!</t>
+  </si>
+  <si>
+    <t>Kalimat aktif: Ayah memotong rumput di halaman,Kalimat pasif: Rumput dipotong oleh ayah di halaman.</t>
+  </si>
+  <si>
+    <t>Jelaskan arti kata "ditemukan"!</t>
+  </si>
+  <si>
+    <t>"Ditemukan" berarti sesuatu yang telah berhasil dilihat atau didapatkan setelah dicari.</t>
+  </si>
+  <si>
+    <t>Buat kalimat dengan kata "ditanam"!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pohon mangga itu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ditanam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oleh kakek di kebun belakang rumah.</t>
+    </r>
+  </si>
+  <si>
+    <t>Apa fungsi awalan "ke-" dalam kata "keempat"?</t>
+  </si>
+  <si>
+    <t>Awalan "ke-" pada kata "keempat" menunjukkan urutan atau bilangan dalam suatu rangkaian.</t>
+  </si>
+  <si>
+    <t>Jelaskan aturan peluluhan huruf pada awalan "me-" dengan contoh!</t>
+  </si>
+  <si>
+    <t>Huruf awal "p" berubah menjadi "mem-": memukul,Huruf awal "t" berubah menjadi "men-": menari,Huruf awal "s" berubah menjadi "meny-": menyapu,Huruf awal "k" berubah menjadi "meng-": mengangkat</t>
+  </si>
+  <si>
+    <t>Tuliskan 3 contoh kata dengan awalan "menge-"!</t>
+  </si>
+  <si>
+    <t>Mengecat, mengejar, mengetuk.</t>
+  </si>
+  <si>
+    <t>Buat paragraf dengan minimal 3 kalimat menggunakan kata berawalan "di-"!</t>
+  </si>
+  <si>
+    <t>Rumah itu dibangun pada tahun 1990. Setiap pagi halamanrumah dibersihkan oleh ibu. Selain itu, tanaman di depan rumah juga disiram setiap sore.</t>
+  </si>
+  <si>
+    <t>Sebutkan contoh kata kerja berawalan "ke-" yang menunjukkan arah!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ke sekolah, ke pantai, ke pasar.</t>
+  </si>
+  <si>
+    <t>Jelaskan arti kata "memasak"!</t>
+  </si>
+  <si>
+    <t>"Memasak" berarti mengolah bahan makanan dengan cara memanaskannya agar bisa dikonsumsi.</t>
+  </si>
+  <si>
+    <t>Buat kalimat yang menunjukkan penggunaan awalan "ke-" sebagai penunjuk urutan!</t>
+  </si>
+  <si>
+    <t>Tim kami berhasil meraih posisi ketiga dalam lomba futsal.</t>
+  </si>
+  <si>
+    <t>Tuliskan contoh kalimat dengan kata "dibawa"!</t>
+  </si>
+  <si>
+    <t>Makanan itu dibawa oleh ibu ke rumah nenek.</t>
+  </si>
+  <si>
+    <t>Sebutkan fungsi awalan "di-" selain menunjukkan tempat!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Menunjukkan tindakan yang diterima oleh subjek, contohnya: Buku itu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dibaca</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oleh siswa.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jelaskan perbedaan makna antara "memasang" dan "dipasang"!</t>
+  </si>
+  <si>
+    <t>"Memasang" berarti melakukan tindakan untuk menempatkan sesuatu di tempat tertentu (kalimat aktif),"Dipasang" berarti menerima tindakan pemasangan oleh subjek (kalimat pasif).</t>
+  </si>
+  <si>
+    <t>Buat paragraf pendek dengan penggunaan awalan "ke-" yang menunjukkan bilangan!</t>
+  </si>
+  <si>
+    <t>Dalam perlombaan itu, saya mendapatkan posisi kedua. Teman saya berada di posisi ketiga, sementara lawan kami berhasil menjadi keempat. Semua peserta berlomba dengan sangat sportif.</t>
+  </si>
+  <si>
+    <t>elaskan penggunaan awalan "meny-" dalam kalimat!</t>
+  </si>
+  <si>
+    <t>Awalan "meny-" digunakan pada kata yang dimulai dengan huruf "s" yang luluh. Contoh: "menyapu" (dari sapu).</t>
+  </si>
+  <si>
+    <t>Berikan contoh kata berawalan "mem-" yang tidak mengalami peluluhan huruf!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Membeli, membangun, memimpin.</t>
+  </si>
+  <si>
+    <t>Sebutkan aturan penggunaan awalan "di-" dalam kalimat pasif!</t>
+  </si>
+  <si>
+    <t>Awalan "di-" digunakan jika subjek menerima tindakan. Biasanya subjek berada di belakang atau tidak disebutkan.</t>
+  </si>
+  <si>
+    <t>Buat kalimat dengan awalan "ke-" yang menunjukkan tujuan perjalanan!</t>
+  </si>
+  <si>
+    <t>Kami akan pergi ke pantai saat liburan nanti.</t>
+  </si>
+  <si>
+    <t>Jelaskan arti kata "diletakkan"!</t>
+  </si>
+  <si>
+    <t>"Diletakkan" berarti menempatkan sesuatu di suatu tempat dan menerima tindakan tersebut (bersifat pasif).</t>
+  </si>
+  <si>
+    <t>Tuliskan contoh kalimat dengan awalan "di-" dan "me-" dalam satu paragraf!</t>
+  </si>
+  <si>
+    <t>Kakak sedang memasak di dapur. Ayah dibantu oleh adik membersihkan halaman. Sementara itu, ibu membaca majalah di ruang tamu.</t>
+  </si>
+  <si>
+    <t>Jelaskan perbedaan penggunaan awalan "ke-" dan "di-" dalam konteks tempat!</t>
+  </si>
+  <si>
+    <t>"ke-" menunjukkan arah atau tujuan (contoh: ke pasar),"di-" menunjukkan posisi tetap atau tempat (contoh: di rumah).</t>
+  </si>
+  <si>
+    <t>Buat kalimat dengan kata "mengecat"!</t>
+  </si>
+  <si>
+    <t>Kami sedang mengecat pagar rumah menjadi warna biru.</t>
+  </si>
+  <si>
+    <t>Sebutkan fungsi awalan "me-" dalam kalimat aktif!</t>
+  </si>
+  <si>
+    <t>Menyatakan bahwa subjek melakukan suatu tindakan atau aktivitas.</t>
+  </si>
+  <si>
+    <t>Tuliskan 3 contoh kalimat menggunakan kata dengan awalan "di-" yang bersifat pasif!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Surat itu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ditulis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oleh Dina,Buku tersebut dipinjam oleh Budi,Makanan tadi dimakan oleh adik.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jelaskan bagaimana aturan perubahan awalan "me-" pada kata yang dimulai dengan huruf "k"!</t>
+  </si>
+  <si>
+    <t>Awalan "me-" berubah menjadi "meng-" apabila huruf awal kata dasar adalah "k" dan huruf "k" luluh. Contoh: "mengangkat" (dari kata dasar "angkat").</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan teks lisan?</t>
+  </si>
+  <si>
+    <t>Teks lisan adalah teks yang disampaikan secara langsung dengan menggunakan suara atau berbicara, bukan dalam bentuk tulisan.</t>
+  </si>
+  <si>
+    <t>Sebutkan 2 contoh situasi yang menggunakan teks lisan!</t>
+  </si>
+  <si>
+    <t>Saat guru memberikan penjelasan di kelas dan saat teman berbicara di depan kelas.</t>
+  </si>
+  <si>
+    <t>Apa perbedaan antara teks lisan dan teks tulisan?</t>
+  </si>
+  <si>
+    <t>Teks lisan disampaikan secara langsung dengan suara,Teks tulisan disampaikan dalam bentuk tulisan yang dapat dibaca.</t>
+  </si>
+  <si>
+    <t>Mengapa mendengarkan teks lisan penting?</t>
+  </si>
+  <si>
+    <t>Karena membantu kita memahami informasi yang disampaikan secara langsung.</t>
+  </si>
+  <si>
+    <t>Apa yang harus diperhatikan saat menyampaikan teks lisan?</t>
+  </si>
+  <si>
+    <t>Intonasi, pelafalan, volume suara, dan kontak mata.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara memahami isi teks lisan dengan baik?</t>
+  </si>
+  <si>
+    <t>Dengan mendengarkan secara saksama dan mencatat hal-hal penting.</t>
+  </si>
+  <si>
+    <t>Sebutkan 3 situasi yang memerlukan teks lisan formal!</t>
+  </si>
+  <si>
+    <t>Pidato, presentasi di sekolah, dan wawancara resmi.</t>
+  </si>
+  <si>
+    <t>Apa yang harus diperhatikan saat mendengarkan teks lisan?</t>
+  </si>
+  <si>
+    <t>Fokus pada isi pembicaraan dan memahami pesan yang disampaikan.</t>
+  </si>
+  <si>
+    <t>Mengapa intonasi penting dalam teks lisan?</t>
+  </si>
+  <si>
+    <t>Karena intonasi dapat membantu pendengar memahami maksud dari pembicara.</t>
+  </si>
+  <si>
+    <t>Sebutkan 2 kesalahan umum dalam menyampaikan teks lisan!</t>
+  </si>
+  <si>
+    <t>Berbicara terlalu cepat dan suara yang terlalu pelan.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan gagasan pokok?</t>
+  </si>
+  <si>
+    <t>Gagasan pokok adalah ide utama yang menjadi inti pembahasan dalam sebuah paragraf.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan gagasan pendukung?</t>
+  </si>
+  <si>
+    <t>Gagasan pendukung adalah ide tambahan yang menjelaskan atau memperkuat gagasan pokok.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara menemukan gagasan pokok dalam sebuah paragraf?</t>
+  </si>
+  <si>
+    <t>Dengan mencari kalimat utama yang biasanya berada di awal, tengah, atau akhir paragraf.</t>
+  </si>
+  <si>
+    <t>Sebutkan perbedaan antara gagasan pokok dan gagasan pendukung!</t>
+  </si>
+  <si>
+    <t>Gagasan pokok adalah ide utama dalam paragraf,Gagasan pendukung menjelaskan atau memperkuat gagasan pokok.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan teks prosedur?</t>
+  </si>
+  <si>
+    <t>Teks prosedur adalah teks yang berisi langkah-langkah atau tahapan untuk melakukan sesuatu.</t>
+  </si>
+  <si>
+    <t>Sebutkan 3 contoh teks prosedur!</t>
+  </si>
+  <si>
+    <t>Cara membuat nasi goreng, cara menanam bunga, dan cara mencuci tangan dengan benar.</t>
+  </si>
+  <si>
+    <t>Apa tujuan dari teks prosedur?</t>
+  </si>
+  <si>
+    <t>Untuk memberikan panduan atau petunjuk melakukan sesuatu dengan benar.</t>
+  </si>
+  <si>
+    <t>Apa yang harus ada dalam teks prosedur?</t>
+  </si>
+  <si>
+    <t>Tujuan, bahan atau alat, serta langkah-langkah.</t>
+  </si>
+  <si>
+    <t>Mengapa teks prosedur penting dalam kehidupan sehari-hari?</t>
+  </si>
+  <si>
+    <t>Karena membantu kita melakukan sesuatu dengan benar dan terstruktur.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara menulis teks prosedur yang baik?</t>
+  </si>
+  <si>
+    <t>Menyusun langkah-langkah secara berurutan dan jelas.</t>
+  </si>
+  <si>
+    <t>Apa yang terjadi jika teks prosedur tidak diikuti dengan benar?</t>
+  </si>
+  <si>
+    <t>Hasil yang didapat tidak sesuai atau mengalami kegagalan.</t>
+  </si>
+  <si>
+    <t>Sebutkan ciri-ciri teks prosedur!</t>
+  </si>
+  <si>
+    <t>Menggunakan langkah-langkah, kalimat imperatif, dan bersifat informatif.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan kata depan?</t>
+  </si>
+  <si>
+    <t>Kata depan adalah kata yang digunakan untuk menghubungkan kata benda atau kata keterangan dengan kata lainnya dalam kalimat.</t>
+  </si>
+  <si>
+    <t>Sebutkan 3 contoh kata depan!</t>
+  </si>
+  <si>
+    <t>Di, ke, dari.</t>
+  </si>
+  <si>
+    <t>Buat kalimat dengan kata depan "ke"!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ayah pergi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ke pasar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pagi ini.</t>
+    </r>
+  </si>
+  <si>
+    <t>Apa perbedaan penggunaan kata depan "di" dan "ke"?</t>
+  </si>
+  <si>
+    <t>"Di" menunjukkan tempat yang tetap,"Ke" menunjukkan arah atau tujuan.</t>
+  </si>
+  <si>
+    <t>Buat kalimat yang menggunakan kata depan "dari"!</t>
+  </si>
+  <si>
+    <t>Dia baru saja pulang dari sekolah.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan kosakata?</t>
+  </si>
+  <si>
+    <t>Kosakata adalah kumpulan kata yang dimiliki seseorang atau suatu bahasa.</t>
+  </si>
+  <si>
+    <t>Mengapa memperkaya kosakata penting?</t>
+  </si>
+  <si>
+    <t>Agar dapat berkomunikasi dengan lebih baik dan memahami berbagai teks.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan paragraf?</t>
+  </si>
+  <si>
+    <t>Paragraf adalah kumpulan kalimat yang saling berhubungan dan membentuk satu kesatuan pikiran.</t>
+  </si>
+  <si>
+    <t>Sebutkan ciri-ciri paragraf yang baik!</t>
+  </si>
+  <si>
+    <t>Memiliki gagasan pokok, kalimat pendukung, dan kesatuan ide.</t>
+  </si>
+  <si>
+    <t>Apa fungsi kalimat penutup dalam paragraf?</t>
+  </si>
+  <si>
+    <t>Untuk memberikan kesimpulan atau penegasan dari isi paragraf.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara membuat paragraf yang baik dan benar?</t>
+  </si>
+  <si>
+    <t>Dengan menentukan gagasan pokok, menyusun kalimat pendukung, dan menjaga kesinambungan antar kalimat.</t>
+  </si>
+  <si>
+    <t>Apa kelebihan dari teks lisan dibandingkan teks tulisan?</t>
+  </si>
+  <si>
+    <t>Teks lisan lebih cepat untuk disampaikan dan dapat langsung mendapatkan tanggapan dari pendengar.</t>
+  </si>
+  <si>
+    <t>Apa yang harus dilakukan jika tidak memahami teks lisan yang disampaikan?</t>
+  </si>
+  <si>
+    <t>Bertanya kepada pembicara atau meminta penjelasan ulang.</t>
+  </si>
+  <si>
+    <t>Sebutkan 2 ciri teks lisan yang efektif!</t>
+  </si>
+  <si>
+    <t>Suara yang jelas dan struktur pembicaraan yang mudah dipahami.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara menjadi pendengar yang baik dalam teks lisan?</t>
+  </si>
+  <si>
+    <t>Fokus pada pembicaraan, tidak berbicara saat mendengarkan, dan mencatat hal penting jika perlu.</t>
+  </si>
+  <si>
+    <t>Mengapa penggunaan bahasa tubuh penting dalam teks lisan?</t>
+  </si>
+  <si>
+    <t>Karena bahasa tubuh dapat membantu memperjelas pesan yang disampaikan.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara mengatasi rasa gugup saat menyampaikan teks lisan di depan orang banyak?</t>
+  </si>
+  <si>
+    <t>Latihan berbicara, menarik napas dalam, dan menjaga kontak mata dengan audiens.</t>
+  </si>
+  <si>
+    <t>Apa yang terjadi jika suatu paragraf tidak memiliki gagasan pokok?</t>
+  </si>
+  <si>
+    <t>Paragraf menjadi tidak jelas dan sulit dipahami pembaca.</t>
+  </si>
+  <si>
+    <t>Mengapa gagasan pendukung penting dalam sebuah paragraf?</t>
+  </si>
+  <si>
+    <t>Untuk memperjelas dan memperkuat gagasan pokok.</t>
+  </si>
+  <si>
+    <t>Bagaimana ciri kalimat yang mengandung gagasan pokok?</t>
+  </si>
+  <si>
+    <t>Kalimat tersebut mengandung ide utama dan biasanya tidak bergantung pada kalimat lain.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan paragraf deduktif?</t>
+  </si>
+  <si>
+    <t>Paragraf yang gagasan pokoknya terletak di awal paragraf.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan paragraf induktif?</t>
+  </si>
+  <si>
+    <t>Paragraf yang gagasan pokoknya terletak di akhir paragraf.</t>
+  </si>
+  <si>
+    <t>Sebutkan 2 manfaat memahami gagasan pokok dalam sebuah teks!</t>
+  </si>
+  <si>
+    <t>Memudahkan memahami isi teks dan membantu dalam membuat ringkasan.</t>
+  </si>
+  <si>
+    <t>Hasil yang diinginkan tidak tercapai atau terjadi kesalahan.</t>
+  </si>
+  <si>
+    <t>Mengapa kalimat imperatif sering digunakan dalam teks prosedur?</t>
+  </si>
+  <si>
+    <t>Karena teks prosedur berisi perintah atau instruksi.</t>
+  </si>
+  <si>
+    <t>Apa saja bagian penting dalam teks prosedur?</t>
+  </si>
+  <si>
+    <t>Tujuan, alat/bahan, dan langkah-langkah.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara membuat teks prosedur yang jelas dan mudah dipahami?</t>
+  </si>
+  <si>
+    <t>Dengan menyusun langkah-langkah secara berurutan dan menggunakan bahasa yang sederhana.</t>
+  </si>
+  <si>
+    <t>Apa yang harus dilakukan jika langkah dalam teks prosedur tidak jelas?</t>
+  </si>
+  <si>
+    <t>Meminta penjelasan tambahan atau mencari referensi lain.</t>
+  </si>
+  <si>
+    <t>Memberikan panduan atau instruksi agar sesuatu dapat dilakukan dengan benar.</t>
+  </si>
+  <si>
+    <t>Apa yang terjadi jika kata depan tidak digunakan dengan benar dalam kalimat?</t>
+  </si>
+  <si>
+    <t>Kalimat menjadi tidak jelas atau memiliki makna yang salah.</t>
+  </si>
+  <si>
+    <t>Apa fungsi kata depan dalam kalimat?</t>
+  </si>
+  <si>
+    <t>Menghubungkan kata benda atau keterangan dengan kata lainnya.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan kosakata baku?</t>
+  </si>
+  <si>
+    <t>Kosakata yang sesuai dengan kaidah bahasa Indonesia yang benar.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara memperkaya kosakata dengan mudah?</t>
+  </si>
+  <si>
+    <t>Dengan membaca berbagai jenis bacaan dan mencatat kosakata baru.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan homonim? Jelaskan dengan contoh!</t>
+  </si>
+  <si>
+    <t>Homonim adalah kata yang memiliki bentuk dan pelafalan yang sama, tetapi memiliki makna yang berbeda. Contoh: bisa (racun ular) dan bisa (mampu).</t>
+  </si>
+  <si>
+    <t>Bagaimana cara menentukan arti kata homonim dalam sebuah kalimat?</t>
+  </si>
+  <si>
+    <t>Dengan melihat konteks kalimat yang digunakan.</t>
+  </si>
+  <si>
+    <t>Jelaskan perbedaan homonim, homofon, dan homograf!</t>
+  </si>
+  <si>
+    <t>Homonim: Bentuk dan pelafalan sama, makna berbeda (contoh: bisa),Homofon: Pelafalan sama, penulisan dan makna berbeda (contoh: masa dan massa),Homograf: Penulisan sama, pelafalan dan makna berbeda (contoh: apel).</t>
+  </si>
+  <si>
+    <t>Apa perbedaan kalimat transitif dan intransitif? Jelaskan dengan contoh!</t>
+  </si>
+  <si>
+    <t>Kalimat transitif membutuhkan objek (contoh: Adik makan roti),Kalimat intransitif tidak membutuhkan objek (contoh: Ibu tidur siang).</t>
+  </si>
+  <si>
+    <t>Ubah kalimat berikut menjadi kalimat intransitif: "Budi memancing ikan di danau."</t>
+  </si>
+  <si>
+    <t>Budi memancing di danau.</t>
+  </si>
+  <si>
+    <t>Ubah kalimat berikut menjadi kalimat transitif: "Ibu memasak di dapur."</t>
+  </si>
+  <si>
+    <t>Ibu memasak sayur di dapur.</t>
+  </si>
+  <si>
+    <t>Mengapa kalimat intransitif tidak memerlukan objek?</t>
+  </si>
+  <si>
+    <t>Karena kalimat intransitif sudah memiliki makna lengkap tanpa tambahan objek.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara mengenali kalimat transitif dalam sebuah paragraf?</t>
+  </si>
+  <si>
+    <t>Dengan mencari keberadaan kata kerja yang membutuhkan objek sebagai pelengkap kalimat.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan kalimat transitif? Jelaskan!</t>
+  </si>
+  <si>
+    <t>Kalimat transitif adalah kalimat yang membutuhkan objek untuk melengkapi maknanya.</t>
+  </si>
+  <si>
+    <t>Ubah kalimat berikut menjadi kalimat transitif: "Rina menyanyi."</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rina menyanyi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lagu favoritnya.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sebutkan tiga ciri utama kalimat transitif!</t>
+  </si>
+  <si>
+    <t>Mengandung kata kerja yang membutuhkan objek,Objek dapat berupa benda atau orang,Jika objek dihilangkan, kalimat menjadi tidak lengkap.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan kata kerja transitif? Berikan contohnya!</t>
+  </si>
+  <si>
+    <t>Kata kerja transitif adalah kata kerja yang membutuhkan objek. Contoh: menulis, membaca, memasak.</t>
+  </si>
+  <si>
+    <t>Apa yang dimaksud dengan kalimat intransitif? Jelaskan!</t>
+  </si>
+  <si>
+    <t>Kalimat intransitif adalah kalimat yang tidak membutuhkan objek untuk melengkapi maknanya.</t>
+  </si>
+  <si>
+    <t>Tuliskan contoh kalimat intransitif yang menggunakan kata kerja tanpa objek!</t>
+  </si>
+  <si>
+    <t>Ibu beristirahat setelah bekerja.</t>
+  </si>
+  <si>
+    <t>Sebutkan tiga ciri kalimat intransitif!</t>
+  </si>
+  <si>
+    <t>Tidak membutuhkan objek,Mengandung kata kerja yang sudah bermakna lengkap,Dapat memiliki keterangan waktu atau tempat</t>
+  </si>
+  <si>
+    <t>Ubah kalimat berikut menjadi kalimat intransitif: "Andi menulis surat untuk teman."</t>
+  </si>
+  <si>
+    <t>Andi menulis di sore hari.</t>
+  </si>
+  <si>
+    <t>Karena kata kerja dalam kalimat intransitif sudah memiliki makna lengkap tanpa tambahan objek.</t>
+  </si>
+  <si>
+    <t>Tuliskan sebuah kalimat intransitif yang mengandung keterangan waktu!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nenek beristirahat </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>setelah makan siang.</t>
+    </r>
+  </si>
+  <si>
+    <t>Apa yang terjadi jika objek ditambahkan pada kalimat intransitif? Jelaskan dengan contoh!</t>
+  </si>
+  <si>
+    <t>Kalimat menjadi tidak sesuai secara tata bahasa. Contoh: "Nenek tidur meja" menjadi tidak benar.</t>
+  </si>
+  <si>
+    <t>Buat satu kalimat intransitif yang menggunakan keterangan cara!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Adik makan </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dengan lahap.</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuliskan kalimat transitif dengan objek berupa nama orang!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Guru memanggil </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ani</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ke depan kelas.</t>
+    </r>
+  </si>
+  <si>
+    <t>Bagaimana cara memahami instruksi dari audio?</t>
+  </si>
+  <si>
+    <t>Dengarkan audio dengan saksama tanpa gangguan,Fokus pada kata kunci yang penting dalam instruksi,Jika memungkinkan, catat informasi penting yang disebutkan.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara menyampaikan pendapat?</t>
+  </si>
+  <si>
+    <t>Mulailah dengan salam dan perkenalan,Jelaskan pendapat secara jelas dan logis,Berikan alasan yang mendukung pendapat tersebut,Gunakan bahasa yang sopan dan tidak menyerang pihak lain.</t>
+  </si>
+  <si>
+    <t>Bagaimana cara membuat teks narasi menggunakan konjungsi?</t>
+  </si>
+  <si>
+    <t>Tentukan tema dan alur cerita yang ingin ditulis,Gunakan kalimat yang variatif dengan konjungsi yang tepat untuk membuat cerita lebih jelas.</t>
   </si>
 </sst>
 </file>
@@ -505,7 +1312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -513,6 +1320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="58" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="B104" zoomScale="58" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,6 +1983,857 @@
       <c r="A44" t="s">
         <v>86</v>
       </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>182</v>
+      </c>
+      <c r="B117" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>233</v>
+      </c>
+      <c r="B118" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>235</v>
+      </c>
+      <c r="B119" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>237</v>
+      </c>
+      <c r="B120" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>239</v>
+      </c>
+      <c r="B121" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>174</v>
+      </c>
+      <c r="B122" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>246</v>
+      </c>
+      <c r="B125" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>252</v>
+      </c>
+      <c r="B128" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>254</v>
+      </c>
+      <c r="B129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>256</v>
+      </c>
+      <c r="B130" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>258</v>
+      </c>
+      <c r="B131" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>260</v>
+      </c>
+      <c r="B132" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>262</v>
+      </c>
+      <c r="B133" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>264</v>
+      </c>
+      <c r="B134" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>266</v>
+      </c>
+      <c r="B135" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>268</v>
+      </c>
+      <c r="B136" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>270</v>
+      </c>
+      <c r="B137" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>272</v>
+      </c>
+      <c r="B138" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>274</v>
+      </c>
+      <c r="B139" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>280</v>
+      </c>
+      <c r="B142" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>262</v>
+      </c>
+      <c r="B143" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>283</v>
+      </c>
+      <c r="B144" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>285</v>
+      </c>
+      <c r="B145" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>287</v>
+      </c>
+      <c r="B146" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>289</v>
+      </c>
+      <c r="B147" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>291</v>
+      </c>
+      <c r="B148" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>293</v>
+      </c>
+      <c r="B149" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>295</v>
+      </c>
+      <c r="B150" t="s">
+        <v>296</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>